<commit_message>
add solutions for 2020.4.29
</commit_message>
<xml_diff>
--- a/做题记录.xlsx
+++ b/做题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DBF91E-0765-4307-B14E-91AEF1C59865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769E1C6E-2DC2-4BD7-8B44-DCF0524A5722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="112">
   <si>
     <t>做题记录</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -235,14 +235,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10E5M5H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0E0M0H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>百题斩001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,10 +263,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1E0M0H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode-cn.com/problems/shu-zu-zhong-shu-zi-chu-xian-de-ci-shu-lcof/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -292,6 +280,197 @@
   </si>
   <si>
     <t>位运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010. 总持续时间可被 60 整除的歌曲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/partition-array-into-three-parts-with-equal-sum/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/pairs-of-songs-with-total-durations-divisible-by-60/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1013. 将数组分成和相等的三个部分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百题斩003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百题斩004</t>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/partition-array-into-three-parts-with-equal-sum/solution/python-3xian-qiu-ping-jun-zai-fen-duan-qiu-he-by-j/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/pairs-of-songs-with-total-durations-divisible-by-60/solution/python-3gou-zao-yi-60-de-yu-shu-wei-suo-yin-de-shu/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>532. 数组中的K-diff数对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/k-diff-pairs-in-an-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组、双指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/k-diff-pairs-in-an-array/solution/python-3wu-xing-jie-ba-xing-jie-by-jpch89/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E10M5H5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E0M0H0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1095. 山脉数组中查找目标值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020 年 4 月每日一题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>852. 山脉数组的峰顶索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/peak-index-in-a-mountain-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/find-in-mountain-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百题斩005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百题斩006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/peak-index-in-a-mountain-array/solution/python-3liang-chong-yi-xing-jie-er-fen-cha-zhao-by/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/find-in-mountain-array/solution/python-3er-fen-cha-zhao-shi-yong-flag-he-bing-shen/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组、二分查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/find-first-and-last-position-of-element-in-sorted-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>34. 在排序数组中查找元素的第一个和最后一个位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百题斩007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/find-first-and-last-position-of-element-in-sorted-array/solution/python-3er-fen-cha-zhao-target-he-target-1-xian-zh/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1064. 不动点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/fixed-point/solution/python-3enumerate-die-dai-er-fen-cha-zhao-by-jpch8/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/fixed-point/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百题斩008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E6M0H0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +510,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -339,15 +518,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -629,16 +897,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.875" customWidth="1"/>
+    <col min="3" max="3" width="44.625" customWidth="1"/>
     <col min="4" max="4" width="24.375" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
     <col min="7" max="7" width="24.875" customWidth="1"/>
@@ -673,10 +941,10 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -705,10 +973,10 @@
       <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -737,14 +1005,14 @@
       <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -769,14 +1037,14 @@
       <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -825,119 +1093,295 @@
         <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1">
         <v>43949</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="J7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" t="s">
-        <v>61</v>
+      <c r="K7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1">
         <v>43949</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" t="s">
-        <v>53</v>
+      <c r="K8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J9" t="s">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43949</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K9" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" t="s">
-        <v>53</v>
+      <c r="K9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J10" t="s">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43949</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" t="s">
-        <v>53</v>
+      <c r="K10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J11" t="s">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43949</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K11" t="s">
-        <v>52</v>
-      </c>
-      <c r="L11" t="s">
-        <v>53</v>
+      <c r="K11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43950</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43950</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43950</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43950</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -957,8 +1401,22 @@
     <hyperlink ref="G7" r:id="rId12" xr:uid="{B335A868-D290-4954-B44D-5A7EEF65E1D4}"/>
     <hyperlink ref="D8" r:id="rId13" xr:uid="{0D5ED265-AD63-48C8-9BC4-952102D19046}"/>
     <hyperlink ref="G8" r:id="rId14" xr:uid="{B0A5DF39-1843-4030-A453-1864896DCBE9}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{5E779170-64C9-4D04-83EE-224A41358D55}"/>
+    <hyperlink ref="D9" r:id="rId16" xr:uid="{4B34F85B-F229-4454-9620-F5B156F9FDF2}"/>
+    <hyperlink ref="G10" r:id="rId17" xr:uid="{71C3B4C7-79A5-4A61-8B60-D263620F7B2C}"/>
+    <hyperlink ref="G9" r:id="rId18" xr:uid="{F334E06D-9078-43C9-B8F0-8CEA56EDFDF0}"/>
+    <hyperlink ref="D11" r:id="rId19" xr:uid="{57C0B76C-1474-40A7-A547-526944ECE7BE}"/>
+    <hyperlink ref="G11" r:id="rId20" xr:uid="{60AE5DFA-B96C-4DD4-BE49-E7244551611C}"/>
+    <hyperlink ref="D12" r:id="rId21" xr:uid="{9EC5D31E-B01C-4BC2-BD3B-E07416802BDA}"/>
+    <hyperlink ref="G13" r:id="rId22" xr:uid="{2D6B2E65-F6A2-4293-BE32-6672D6CEA51F}"/>
+    <hyperlink ref="G12" r:id="rId23" xr:uid="{97664155-61E7-49B5-85DF-0D9E69CA661B}"/>
+    <hyperlink ref="D13" r:id="rId24" xr:uid="{BAB7298A-73FD-4DD8-B734-AA6582094875}"/>
+    <hyperlink ref="D14" r:id="rId25" xr:uid="{57E3EF05-7FC5-49BF-9E3F-240F11E77A10}"/>
+    <hyperlink ref="G14" r:id="rId26" xr:uid="{10DE1309-194F-4DD8-9035-65D1E9B80D10}"/>
+    <hyperlink ref="G15" r:id="rId27" xr:uid="{25FE67F1-30FF-4021-B9F4-8881181AEBD4}"/>
+    <hyperlink ref="D15" r:id="rId28" xr:uid="{0630F09B-AD39-4A81-823D-D9ECF3A75CC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add JavaScript solution for 226. 翻转二叉树
</commit_message>
<xml_diff>
--- a/做题记录.xlsx
+++ b/做题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC46C83F-F4BC-4F06-98A0-3F912C13A62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BFB71B-F2AF-4F23-81A2-BEE515F84F63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4308,8 +4308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G174" sqref="G174"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6373,7 +6373,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>635</v>
+        <v>840</v>
       </c>
       <c r="B68" s="1">
         <v>43993</v>

</xml_diff>